<commit_message>
Added reserved field handling
</commit_message>
<xml_diff>
--- a/spreadsheets/example_spreadsheet.xlsx
+++ b/spreadsheets/example_spreadsheet.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t xml:space="preserve">GROUP</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t xml:space="preserve">Example field 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESERVED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[31:2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved</t>
   </si>
 </sst>
 </file>
@@ -162,6 +174,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -327,7 +340,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.68"/>
   </cols>
@@ -381,21 +394,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="260" zoomScaleNormal="260" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,6 +567,23 @@
       </c>
       <c r="F9" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>